<commit_message>
now the code reads and executes all of the links on the page
</commit_message>
<xml_diff>
--- a/import_file.xlsx
+++ b/import_file.xlsx
@@ -427,8 +427,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
updated the script to read and execute all of the links on first three pages.
</commit_message>
<xml_diff>
--- a/import_file.xlsx
+++ b/import_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">IBTech Uluslararası Bilişim ve İletişim Teknolojileri
 </t>
@@ -65,6 +65,13 @@
     <t>https://twitter.com</t>
   </si>
   <si>
+    <t xml:space="preserve">IBTech Hackathon &amp; Bootcamp - Coderspace
+</t>
+  </si>
+  <si>
+    <t>https://coderspace.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">IBtech Staj ve İş İlanları &amp; Şirket Kültürü - Youthall
 </t>
   </si>
@@ -72,11 +79,133 @@
     <t>https://www.youthall.com</t>
   </si>
   <si>
-    <t xml:space="preserve">IBTech Hackathon &amp; Bootcamp - Coderspace
-</t>
-  </si>
-  <si>
-    <t>https://coderspace.com</t>
+    <t xml:space="preserve">IBTECH A.S. | LinkedIn
+</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ibtech Bootcamp - Patika
+</t>
+  </si>
+  <si>
+    <t>https://www.patika.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBTech (Turkey) Salaries in Turkey - Glassdoor
+</t>
+  </si>
+  <si>
+    <t>https://www.glassdoor.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ibtech - ITEA 4
+</t>
+  </si>
+  <si>
+    <t>https://itea4.com</t>
+  </si>
+  <si>
+    <t>Ibtech Bilgi İşlem Merkezi Genel Müdürlüğü - Arkiv
+http://www.arkiv.com.tr › proje › ibt...
+·
+Translate this page</t>
+  </si>
+  <si>
+    <t>https://Ibtech Bilgi İşlem Merkezi Genel Müdürlüğü - Arkiv
+http://www.arkiv.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBTECH A.S. - Information Technology &amp; Services - Apollo.io
+</t>
+  </si>
+  <si>
+    <t>https://www.apollo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBTECH - CM Mimarlık
+</t>
+  </si>
+  <si>
+    <t>https://cmmimarlik.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBTEch Staffing
+</t>
+  </si>
+  <si>
+    <t>https://ibtechstaffing.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBTECH ULUSLARARASI BİLİŞİM VE İLETİŞİM ... - Bulurum.com
+</t>
+  </si>
+  <si>
+    <t>https://www.bulurum.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to get to IBTECH in Gebze by Bus or Cable Car?
+</t>
+  </si>
+  <si>
+    <t>https://moovitapp.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBTECH Karekodlu Geçiş Sistemi - Argenova
+</t>
+  </si>
+  <si>
+    <t>https://www.argenova.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBTech Uluslararası Bilişim ve İletişim Teknolojileri - Mind2Biz
+</t>
+  </si>
+  <si>
+    <t>https://www.mind2biz.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBTech Case Study | Micro Focus
+</t>
+  </si>
+  <si>
+    <t>https://www.microfocus.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qnb Finansbank Batı Kule IbTech - Foursquare
+</t>
+  </si>
+  <si>
+    <t>https://foursquare.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gallery of IBTECH IT Center Headquarters / CM Mimarlık - 1
+</t>
+  </si>
+  <si>
+    <t>https://www.archdaily.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBTECH şirketi: Çalışan Yorumları | Indeed.com
+</t>
+  </si>
+  <si>
+    <t>https://tr.indeed.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ibtech - Metin Örnek, MBA, PMP
+</t>
+  </si>
+  <si>
+    <t>https://www.metinornek.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBTECH – QNB Finansbank Created A Smart Orchestration ...
+</t>
+  </si>
+  <si>
+    <t>https://www.infosec.com</t>
   </si>
 </sst>
 </file>
@@ -421,14 +550,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -501,6 +630,150 @@
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -514,6 +787,24 @@
     <hyperlink ref="B7" r:id="rId7"/>
     <hyperlink ref="B8" r:id="rId8"/>
     <hyperlink ref="B9" r:id="rId9"/>
+    <hyperlink ref="B10" r:id="rId10"/>
+    <hyperlink ref="B11" r:id="rId11"/>
+    <hyperlink ref="B12" r:id="rId12"/>
+    <hyperlink ref="B13" r:id="rId13"/>
+    <hyperlink ref="B14" r:id="rId14"/>
+    <hyperlink ref="B15" r:id="rId15"/>
+    <hyperlink ref="B16" r:id="rId16"/>
+    <hyperlink ref="B17" r:id="rId17"/>
+    <hyperlink ref="B18" r:id="rId18"/>
+    <hyperlink ref="B19" r:id="rId19"/>
+    <hyperlink ref="B20" r:id="rId20"/>
+    <hyperlink ref="B21" r:id="rId21"/>
+    <hyperlink ref="B22" r:id="rId22"/>
+    <hyperlink ref="B23" r:id="rId23"/>
+    <hyperlink ref="B24" r:id="rId24"/>
+    <hyperlink ref="B25" r:id="rId25"/>
+    <hyperlink ref="B26" r:id="rId26"/>
+    <hyperlink ref="B27" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>